<commit_message>
New sea otter index for 2018 (Stephens) built
</commit_message>
<xml_diff>
--- a/sea_otter_index_2018/sites_2018_stephens.xlsx
+++ b/sea_otter_index_2018/sites_2018_stephens.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiff/Desktop/R Studio/APECS-master-repos/sea_otter_index_2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E63511-3C5E-8048-8836-3CAA655240E3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A8EF98-6610-A847-852E-9613339A44FB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="0" windowWidth="24680" windowHeight="18700" xr2:uid="{B7656634-A4D9-CB4B-BCBA-A716DC3A2AB6}"/>
+    <workbookView xWindow="12020" yWindow="1220" windowWidth="14120" windowHeight="18700" xr2:uid="{B7656634-A4D9-CB4B-BCBA-A716DC3A2AB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="43">
   <si>
     <t>site</t>
   </si>
@@ -128,6 +128,33 @@
   </si>
   <si>
     <t>survey_date2_MM/DD/YY</t>
+  </si>
+  <si>
+    <t>so_duration</t>
+  </si>
+  <si>
+    <t>pop_dens_surv_km2</t>
+  </si>
+  <si>
+    <t>date_grass_MM.DD.YY</t>
+  </si>
+  <si>
+    <t>date_otts1_MM.DD.YY</t>
+  </si>
+  <si>
+    <t>date_otts2_MM.DD.YY</t>
+  </si>
+  <si>
+    <t>otter_region</t>
+  </si>
+  <si>
+    <t>mid</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>high</t>
   </si>
 </sst>
 </file>
@@ -484,23 +511,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C252BE23-1EDC-7A4D-A693-E082E052B44D}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.1640625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="10.83203125" style="1"/>
-    <col min="4" max="4" width="10.83203125" style="2"/>
-    <col min="5" max="5" width="10.83203125" style="1"/>
-    <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="2" max="5" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -510,17 +537,29 @@
       <c r="C1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -530,17 +569,29 @@
       <c r="C2" s="1">
         <v>55.227691</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="2">
+        <v>43294</v>
+      </c>
+      <c r="F2" s="2">
         <v>43299</v>
       </c>
-      <c r="E2" s="2">
+      <c r="G2" s="2">
         <v>43307</v>
       </c>
-      <c r="F2" s="1">
+      <c r="H2" s="1">
         <v>6.4850000000000003</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I2" s="1">
+        <v>7</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -550,17 +601,29 @@
       <c r="C3" s="1">
         <v>55.585855000000002</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="2">
+        <v>43292</v>
+      </c>
+      <c r="F3" s="2">
         <v>43300</v>
       </c>
-      <c r="E3" s="2">
+      <c r="G3" s="2">
         <v>43313</v>
       </c>
-      <c r="F3" s="1">
+      <c r="H3" s="1">
         <v>13.8025</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I3" s="1">
+        <v>14</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1.341</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -570,17 +633,29 @@
       <c r="C4" s="1">
         <v>55.621174000000003</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="2">
+        <v>43269</v>
+      </c>
+      <c r="F4" s="2">
         <v>43276</v>
       </c>
-      <c r="E4" s="2">
+      <c r="G4" s="2">
         <v>43317</v>
       </c>
-      <c r="F4" s="1">
+      <c r="H4" s="1">
         <v>14.577500000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I4" s="1">
+        <v>14</v>
+      </c>
+      <c r="J4">
+        <v>2.8769999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -590,17 +665,29 @@
       <c r="C5" s="1">
         <v>55.813558</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="2">
+        <v>43264</v>
+      </c>
+      <c r="F5" s="2">
         <v>43258</v>
       </c>
-      <c r="E5" s="2">
+      <c r="G5" s="2">
         <v>43308</v>
       </c>
-      <c r="F5" s="1">
+      <c r="H5" s="1">
         <v>12.57</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I5" s="1">
+        <v>14</v>
+      </c>
+      <c r="J5">
+        <v>2.8769999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -610,17 +697,29 @@
       <c r="C6" s="1">
         <v>55.084800000000001</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="2">
+        <v>43323</v>
+      </c>
+      <c r="F6" s="2">
         <v>43305</v>
       </c>
-      <c r="E6" s="2">
+      <c r="G6" s="2">
         <v>43322</v>
       </c>
-      <c r="F6" s="1">
+      <c r="H6" s="1">
         <v>9.44</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I6" s="1">
+        <v>7</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -630,17 +729,29 @@
       <c r="C7" s="1">
         <v>55.552180999999997</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="2">
+        <v>43293</v>
+      </c>
+      <c r="F7" s="2">
         <v>43243</v>
       </c>
-      <c r="E7" s="2">
+      <c r="G7" s="2">
         <v>43306</v>
       </c>
-      <c r="F7" s="1">
+      <c r="H7" s="1">
         <v>10.057499999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I7" s="1">
+        <v>14</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1.341</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -650,17 +761,29 @@
       <c r="C8" s="1">
         <v>55.192860000000003</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="2">
+        <v>43265</v>
+      </c>
+      <c r="F8" s="2">
         <v>43263</v>
       </c>
-      <c r="E8" s="2">
+      <c r="G8" s="2">
         <v>43307</v>
       </c>
-      <c r="F8" s="1">
+      <c r="H8" s="1">
         <v>4.4924999999999997</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I8" s="1">
+        <v>7</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -670,17 +793,29 @@
       <c r="C9" s="1">
         <v>55.740264000000003</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="2">
+        <v>43251</v>
+      </c>
+      <c r="F9" s="2">
         <v>43257</v>
       </c>
-      <c r="E9" s="2">
+      <c r="G9" s="2">
         <v>43312</v>
       </c>
-      <c r="F9" s="1">
+      <c r="H9" s="1">
         <v>8.33</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I9" s="1">
+        <v>14</v>
+      </c>
+      <c r="J9">
+        <v>2.8769999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -690,17 +825,29 @@
       <c r="C10" s="1">
         <v>55.865721000000001</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="2">
+        <v>43249</v>
+      </c>
+      <c r="F10" s="2">
         <v>43257</v>
       </c>
-      <c r="E10" s="2">
+      <c r="G10" s="2">
         <v>43312</v>
       </c>
-      <c r="F10" s="1">
+      <c r="H10" s="1">
         <v>11.352499999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I10" s="1">
+        <v>14</v>
+      </c>
+      <c r="J10">
+        <v>2.8769999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -710,17 +857,29 @@
       <c r="C11" s="1">
         <v>55.733423000000002</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="2">
+        <v>43250</v>
+      </c>
+      <c r="F11" s="2">
         <v>43257</v>
       </c>
-      <c r="E11" s="2">
+      <c r="G11" s="2">
         <v>43312</v>
       </c>
-      <c r="F11" s="1">
+      <c r="H11" s="1">
         <v>6.7450000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I11" s="1">
+        <v>14</v>
+      </c>
+      <c r="J11">
+        <v>2.8769999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -730,17 +889,29 @@
       <c r="C12" s="1">
         <v>55.889904000000001</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="2">
+        <v>43295</v>
+      </c>
+      <c r="F12" s="2">
         <v>43258</v>
       </c>
-      <c r="E12" s="2">
+      <c r="G12" s="2">
         <v>43317</v>
       </c>
-      <c r="F12" s="1">
+      <c r="H12" s="1">
         <v>10.41</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I12" s="1">
+        <v>14</v>
+      </c>
+      <c r="J12">
+        <v>2.8769999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -750,17 +921,29 @@
       <c r="C13" s="1">
         <v>55.214374999999997</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="2">
+        <v>43267</v>
+      </c>
+      <c r="F13" s="2">
         <v>43263</v>
       </c>
-      <c r="E13" s="2">
+      <c r="G13" s="2">
         <v>43307</v>
       </c>
-      <c r="F13" s="1">
+      <c r="H13" s="1">
         <v>17.635000000000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I13" s="1">
+        <v>7</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0.154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
@@ -770,17 +953,29 @@
       <c r="C14" s="1">
         <v>55.496471999999997</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="2">
+        <v>43279</v>
+      </c>
+      <c r="F14" s="2">
         <v>43290</v>
       </c>
-      <c r="E14" s="2">
+      <c r="G14" s="2">
         <v>43320</v>
       </c>
-      <c r="F14" s="1">
+      <c r="H14" s="1">
         <v>15.49</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I14" s="1">
+        <v>14</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1.341</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -790,17 +985,29 @@
       <c r="C15" s="1">
         <v>55.247539000000003</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="2">
+        <v>43266</v>
+      </c>
+      <c r="F15" s="2">
         <v>43263</v>
       </c>
-      <c r="E15" s="2">
+      <c r="G15" s="2">
         <v>43307</v>
       </c>
-      <c r="F15" s="1">
+      <c r="H15" s="1">
         <v>13.15</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I15" s="1">
+        <v>7</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0.154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -810,17 +1017,29 @@
       <c r="C16" s="1">
         <v>55.241886999999998</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="2">
+        <v>43267</v>
+      </c>
+      <c r="F16" s="2">
         <v>43263</v>
       </c>
-      <c r="E16" s="2">
+      <c r="G16" s="2">
         <v>43307</v>
       </c>
-      <c r="F16" s="1">
+      <c r="H16" s="1">
         <v>15.03</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I16" s="1">
+        <v>7</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0.154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -830,17 +1049,29 @@
       <c r="C17" s="1">
         <v>55.228251999999998</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="2">
+        <v>43266</v>
+      </c>
+      <c r="F17" s="2">
         <v>43263</v>
       </c>
-      <c r="E17" s="2">
+      <c r="G17" s="2">
         <v>43307</v>
       </c>
-      <c r="F17" s="1">
+      <c r="H17" s="1">
         <v>8.1724999999999994</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I17" s="1">
+        <v>7</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0.154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -850,17 +1081,29 @@
       <c r="C18" s="1">
         <v>55.709094</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="2">
+        <v>43239</v>
+      </c>
+      <c r="F18" s="2">
         <v>43225</v>
       </c>
-      <c r="E18" s="2">
+      <c r="G18" s="2">
         <v>43317</v>
       </c>
-      <c r="F18" s="1">
+      <c r="H18" s="1">
         <v>6.4024999999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I18" s="1">
+        <v>14</v>
+      </c>
+      <c r="J18">
+        <v>2.8769999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
@@ -870,17 +1113,29 @@
       <c r="C19" s="1">
         <v>55.722636999999999</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="2">
+        <v>43281</v>
+      </c>
+      <c r="F19" s="2">
         <v>43225</v>
       </c>
-      <c r="E19" s="2">
+      <c r="G19" s="2">
         <v>43317</v>
       </c>
-      <c r="F19" s="1">
+      <c r="H19" s="1">
         <v>7.4349999999999996</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I19" s="1">
+        <v>14</v>
+      </c>
+      <c r="J19">
+        <v>2.8769999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -890,17 +1145,29 @@
       <c r="C20" s="1">
         <v>55.362090000000002</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="2">
+        <v>43291</v>
+      </c>
+      <c r="F20" s="2">
         <v>43290</v>
       </c>
-      <c r="E20" s="2">
+      <c r="G20" s="2">
         <v>43307</v>
       </c>
-      <c r="F20" s="1">
+      <c r="H20" s="1">
         <v>5.83</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I20" s="1">
+        <v>7</v>
+      </c>
+      <c r="J20" s="1">
+        <v>1.341</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -910,17 +1177,29 @@
       <c r="C21" s="1">
         <v>55.282136999999999</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="2">
+        <v>43322</v>
+      </c>
+      <c r="F21" s="2">
         <v>43305</v>
       </c>
-      <c r="E21" s="2">
+      <c r="G21" s="2">
         <v>43326</v>
       </c>
-      <c r="F21" s="1">
+      <c r="H21" s="1">
         <v>5.0250000000000004</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I21" s="1">
+        <v>7</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0.154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -930,17 +1209,29 @@
       <c r="C22" s="1">
         <v>55.485686999999999</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="2">
+        <v>43276</v>
+      </c>
+      <c r="F22" s="2">
         <v>43290</v>
       </c>
-      <c r="E22" s="2">
+      <c r="G22" s="2">
         <v>43320</v>
       </c>
-      <c r="F22" s="1">
+      <c r="H22" s="1">
         <v>24.272500000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I22" s="1">
+        <v>14</v>
+      </c>
+      <c r="J22" s="1">
+        <v>1.341</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -950,17 +1241,29 @@
       <c r="C23" s="1">
         <v>55.528424000000001</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="2">
+        <v>43263</v>
+      </c>
+      <c r="F23" s="2">
         <v>43262</v>
       </c>
-      <c r="E23" s="2">
+      <c r="G23" s="2">
         <v>43315</v>
       </c>
-      <c r="F23" s="1">
+      <c r="H23" s="1">
         <v>20.6</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I23" s="1">
+        <v>14</v>
+      </c>
+      <c r="J23" s="1">
+        <v>1.341</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>11</v>
       </c>
@@ -970,17 +1273,29 @@
       <c r="C24" s="1">
         <v>55.684275</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="2">
+        <v>43238</v>
+      </c>
+      <c r="F24" s="2">
         <v>43227</v>
       </c>
-      <c r="E24" s="2">
+      <c r="G24" s="2">
         <v>43293</v>
       </c>
-      <c r="F24" s="1">
+      <c r="H24" s="1">
         <v>12.49</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I24" s="1">
+        <v>14</v>
+      </c>
+      <c r="J24">
+        <v>2.8769999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
@@ -990,17 +1305,29 @@
       <c r="C25" s="1">
         <v>55.599083</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="2">
+        <v>43268</v>
+      </c>
+      <c r="F25" s="2">
         <v>43296</v>
       </c>
-      <c r="E25" s="2">
+      <c r="G25" s="2">
         <v>43313</v>
       </c>
-      <c r="F25" s="1">
+      <c r="H25" s="1">
         <v>11.335000000000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I25" s="1">
+        <v>14</v>
+      </c>
+      <c r="J25" s="1">
+        <v>1.341</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -1010,17 +1337,29 @@
       <c r="C26" s="1">
         <v>55.264232</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="2">
+        <v>43278</v>
+      </c>
+      <c r="F26" s="2">
         <v>43299</v>
       </c>
-      <c r="E26" s="2">
+      <c r="G26" s="2">
         <v>43310</v>
       </c>
-      <c r="F26" s="1">
+      <c r="H26" s="1">
         <v>9.52</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I26" s="1">
+        <v>7</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0.154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -1030,18 +1369,30 @@
       <c r="C27" s="1">
         <v>55.188785000000003</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" s="2">
+        <v>43265</v>
+      </c>
+      <c r="F27" s="2">
         <v>43263</v>
       </c>
-      <c r="E27" s="2">
+      <c r="G27" s="2">
         <v>43307</v>
       </c>
-      <c r="F27" s="1">
+      <c r="H27" s="1">
         <v>13.8775</v>
       </c>
+      <c r="I27" s="1">
+        <v>7</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0.154</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F27">
+  <sortState ref="A2:H27">
     <sortCondition ref="A2:A27"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Wrote a bunch of new code to build the first wave of analysis on the elevation data. HTML file looking good.
</commit_message>
<xml_diff>
--- a/sea_otter_index_2018/sites_2018_stephens.xlsx
+++ b/sea_otter_index_2018/sites_2018_stephens.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiff/Desktop/R Studio/APECS-master-repos/sea_otter_index_2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A8EF98-6610-A847-852E-9613339A44FB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F2F555-8D28-8D4C-AF23-52C70CA8ECDC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12020" yWindow="1220" windowWidth="14120" windowHeight="18700" xr2:uid="{B7656634-A4D9-CB4B-BCBA-A716DC3A2AB6}"/>
+    <workbookView xWindow="12020" yWindow="1220" windowWidth="18960" windowHeight="14760" xr2:uid="{B7656634-A4D9-CB4B-BCBA-A716DC3A2AB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -514,7 +514,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -747,8 +747,8 @@
       <c r="I7" s="1">
         <v>14</v>
       </c>
-      <c r="J7" s="1">
-        <v>1.341</v>
+      <c r="J7">
+        <v>2.8769999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -1392,7 +1392,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:H27">
+  <sortState ref="A2:J27">
     <sortCondition ref="A2:A27"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>